<commit_message>
done: add email to fetch employee
</commit_message>
<xml_diff>
--- a/src/scripts/employees.xlsx
+++ b/src/scripts/employees.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>employee_id</t>
   </si>
@@ -26,7 +26,7 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>aadhar_link</t>
+    <t>email</t>
   </si>
   <si>
     <t>whatsapp_number</t>
@@ -50,7 +50,7 @@
     <t>shitole</t>
   </si>
   <si>
-    <t>https://aadhar.gov.in/emp01</t>
+    <t>dummy@email.com</t>
   </si>
   <si>
     <t>dsfd7d8df</t>
@@ -71,9 +71,6 @@
     <t>Somwanshi</t>
   </si>
   <si>
-    <t>https://aadhar.gov.in/emp02</t>
-  </si>
-  <si>
     <t>dsfd7d8sdsdf</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>biradar</t>
   </si>
   <si>
-    <t>https://aadhar.gov.in/emp03</t>
-  </si>
-  <si>
     <t>dsfwewewd7d8df</t>
   </si>
   <si>
@@ -104,9 +98,6 @@
     <t>patil</t>
   </si>
   <si>
-    <t>https://aadhar.gov.in/emp05</t>
-  </si>
-  <si>
     <t>dsfsdsad7d8df</t>
   </si>
   <si>
@@ -119,9 +110,6 @@
     <t>alur</t>
   </si>
   <si>
-    <t>https://aadhar.gov.in/emp06</t>
-  </si>
-  <si>
     <t>w2ddd</t>
   </si>
   <si>
@@ -135,9 +123,6 @@
   </si>
   <si>
     <t>agrawal</t>
-  </si>
-  <si>
-    <t>https://aadhar.gov.in/emp04</t>
   </si>
   <si>
     <t>casda</t>
@@ -244,7 +229,7 @@
     <tableColumn name="employee_id" id="1"/>
     <tableColumn name="first_name" id="2"/>
     <tableColumn name="last_name" id="3"/>
-    <tableColumn name="aadhar_link" id="4"/>
+    <tableColumn name="email" id="4"/>
     <tableColumn name="whatsapp_number" id="5"/>
     <tableColumn name="uuid" id="6"/>
     <tableColumn name="is_qr_sent" id="7"/>
@@ -551,7 +536,7 @@
     <col min="1" max="1" style="5" width="13.862142857142858" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="35.005" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="7" width="19.290714285714284" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -621,13 +606,13 @@
         <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>8830427235</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>13</v>
@@ -638,106 +623,106 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3">
         <v>9075072341</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="E5" s="3">
         <v>6354107850</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="E6" s="3">
         <v>8530797631</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3">
         <v>907552949098</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>